<commit_message>
msz - repplacing AppiumLibrary by native python-appium-client (part 1)
</commit_message>
<xml_diff>
--- a/Data/Pages/dlgAutomobileInsurance_pagProductData.xlsx
+++ b/Data/Pages/dlgAutomobileInsurance_pagProductData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C5A535-7A34-4041-A79A-E59E93FD1322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F8920-F103-45D7-881D-AE2F0B4DCBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1608" windowWidth="36948" windowHeight="15672" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3444" yWindow="1248" windowWidth="35136" windowHeight="13680" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>